<commit_message>
localized dec point and thousand separator
</commit_message>
<xml_diff>
--- a/tests/issues_format_date_currency.xlsx
+++ b/tests/issues_format_date_currency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/supplyframe/rsbom/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E41942-9934-B24C-8788-3E00F62DE0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABB657A-5F79-9A47-9D6A-CE1B36A0F837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="5140" windowWidth="26040" windowHeight="14940" xr2:uid="{BA8D3F58-9B48-4943-9244-C0B8A4673576}"/>
+    <workbookView xWindow="8220" yWindow="5740" windowWidth="26040" windowHeight="14940" xr2:uid="{BA8D3F58-9B48-4943-9244-C0B8A4673576}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,18 +37,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-407]d/\ mmm/\ yy;@"/>
-    <numFmt numFmtId="168" formatCode="[$-1004]dddd\,\ d\ mmmm\,\ yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-407]mmmm\ yy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-404]aaa;@"/>
-    <numFmt numFmtId="174" formatCode="[$-407]d/\ mmm/;@"/>
-    <numFmt numFmtId="175" formatCode="d/m/yy\ h:mm;@"/>
-    <numFmt numFmtId="178" formatCode="#.##000"/>
+  <numFmts count="12">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-407]d/\ mmm/\ yy;@"/>
+    <numFmt numFmtId="169" formatCode="[$-1004]dddd\,\ d\ mmmm\,\ yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-407]mmmm\ yy;@"/>
+    <numFmt numFmtId="171" formatCode="[$-404]aaa;@"/>
+    <numFmt numFmtId="172" formatCode="[$-407]d/\ mmm/;@"/>
+    <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="175" formatCode="[$XOF]\ #,##0.00_);\([$XOF]\ #,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ [$F CFA-340C];\-#,##0.00\ [$F CFA-340C]"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,19 +82,19 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +412,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,10 +476,14 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+      <c r="A12" s="12">
+        <v>2341234</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
+      <c r="A13" s="13">
+        <v>2341234</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
string value formating fix
</commit_message>
<xml_diff>
--- a/tests/issues_format_date_currency.xlsx
+++ b/tests/issues_format_date_currency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/supplyframe/rsbom/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABB657A-5F79-9A47-9D6A-CE1B36A0F837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB5F256-C1D6-E448-B35D-97EDD4120BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8220" yWindow="5740" windowWidth="26040" windowHeight="14940" xr2:uid="{BA8D3F58-9B48-4943-9244-C0B8A4673576}"/>
   </bookViews>
@@ -35,21 +35,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>2/28/2024</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="12">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="168" formatCode="[$-407]d/\ mmm/\ yy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-1004]dddd\,\ d\ mmmm\,\ yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-407]mmmm\ yy;@"/>
-    <numFmt numFmtId="171" formatCode="[$-404]aaa;@"/>
-    <numFmt numFmtId="172" formatCode="[$-407]d/\ mmm/;@"/>
-    <numFmt numFmtId="173" formatCode="d/m/yy\ h:mm;@"/>
-    <numFmt numFmtId="175" formatCode="[$XOF]\ #,##0.00_);\([$XOF]\ #,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00\ [$F CFA-340C];\-#,##0.00\ [$F CFA-340C]"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-407]d/\ mmm/\ yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-1004]dddd\,\ d\ mmmm\,\ yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="[$-407]mmmm\ yy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-404]aaa;@"/>
+    <numFmt numFmtId="171" formatCode="[$-407]d/\ mmm/;@"/>
+    <numFmt numFmtId="172" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="173" formatCode="[$XOF]\ #,##0.00_);\([$XOF]\ #,##0.00\)"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ [$F CFA-340C];\-#,##0.00\ [$F CFA-340C]"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -68,7 +76,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,25 +84,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCD89B7-6E06-DB4B-9F33-1A336288FE31}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,6 +511,11 @@
         <v>2341234</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>